<commit_message>
- Eliminated nodes that have not been created yet
</commit_message>
<xml_diff>
--- a/TorpedoBackend/Agent/Graph.xlsx
+++ b/TorpedoBackend/Agent/Graph.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Arad</t>
   </si>
@@ -31,16 +31,10 @@
     <t xml:space="preserve">(Zerind, 75, 50, 10.2)</t>
   </si>
   <si>
-    <t xml:space="preserve">(Sibiu, 140, 50, 11)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Timisoara</t>
   </si>
   <si>
     <t xml:space="preserve">(Arad, 118, 50, 10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Lugo, 111, 60, 9)</t>
   </si>
   <si>
     <t xml:space="preserve">Zerind</t>
@@ -61,6 +55,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,7 +137,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
@@ -166,27 +161,21 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Updated Graph.xlsx to include straight line distance (heuristic value). 2. Updated GraphInput->sheetImport() to assign the new heuristic values from the updated Graph.xlsx to the proper Node. 3. Tester for Simulated Annealing.
</commit_message>
<xml_diff>
--- a/TorpedoBackend/Agent/Graph.xlsx
+++ b/TorpedoBackend/Agent/Graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oatorresdiaz/Documents/Torpedo/TorpedoBackend/Agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FD5331-CFB6-C042-9CF3-37EFE797509F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D40628-B2B8-3D46-AF82-D4FAAC0510BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="21960" windowHeight="13560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="10000" windowHeight="13560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,18 +96,12 @@
     <t>Vaslui</t>
   </si>
   <si>
-    <t>lasi</t>
-  </si>
-  <si>
     <t>Neamt</t>
   </si>
   <si>
     <t>Hirsova</t>
   </si>
   <si>
-    <t>Efo rie</t>
-  </si>
-  <si>
     <t>(Timisoara, 111, 50, 13.4)</t>
   </si>
   <si>
@@ -198,24 +192,15 @@
     <t>(Urziceni, 142, 50, 13.4)</t>
   </si>
   <si>
-    <t>(lasi, 92, 50, 13.4)</t>
-  </si>
-  <si>
     <t>(Vaslui, 92, 50, 13.4)</t>
   </si>
   <si>
     <t>(Neamt, 87, 50, 13.4)</t>
   </si>
   <si>
-    <t>(lasi, 87, 50, 13.4)</t>
-  </si>
-  <si>
     <t>(Urziceni, 98, 50, 13.4)</t>
   </si>
   <si>
-    <t>(Efo rie, 86, 50, 13.4)</t>
-  </si>
-  <si>
     <t>(Hirsova, 86, 50, 13.4)</t>
   </si>
   <si>
@@ -223,6 +208,21 @@
   </si>
   <si>
     <t>Giurgiu</t>
+  </si>
+  <si>
+    <t>(Eforie, 86, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>Eforie</t>
+  </si>
+  <si>
+    <t>Iasi</t>
+  </si>
+  <si>
+    <t>(Iasi, 87, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(Iasi, 92, 50, 13.4)</t>
   </si>
 </sst>
 </file>
@@ -586,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -602,242 +602,302 @@
     <col min="6" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>366</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>329</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>374</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>380</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>27</v>
+      <c r="B5">
+        <v>244</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
+      <c r="B6">
+        <v>241</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>31</v>
+      <c r="B7">
+        <v>242</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>160</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>193</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>253</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>43</v>
+      <c r="B11">
+        <v>176</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <v>199</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17">
+        <v>226</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>234</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>151</v>
+      </c>
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20">
+        <v>161</v>
+      </c>
+      <c r="C20" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created new map on a new sheet: Map_2.
</commit_message>
<xml_diff>
--- a/TorpedoBackend/Agent/Graph.xlsx
+++ b/TorpedoBackend/Agent/Graph.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oatorresdiaz/Documents/Torpedo/TorpedoBackend/Agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D40628-B2B8-3D46-AF82-D4FAAC0510BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF712DA-0640-E94D-961E-B52AC98226FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="10000" windowHeight="13560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18900" yWindow="4060" windowWidth="17120" windowHeight="13560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Romania" sheetId="1" r:id="rId1"/>
+    <sheet name="Map 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="130">
   <si>
     <t>Arad</t>
   </si>
@@ -223,6 +224,198 @@
   </si>
   <si>
     <t>(Iasi, 92, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>(B, 118, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(C, 75, 50, 10.2)</t>
+  </si>
+  <si>
+    <t>(D, 140, 50, 11)</t>
+  </si>
+  <si>
+    <t>(A, 118, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>E, 75, 50, 10.2)</t>
+  </si>
+  <si>
+    <t>(G, 140, 50, 11)</t>
+  </si>
+  <si>
+    <t>(F, 75, 50, 10.2)</t>
+  </si>
+  <si>
+    <t>(K, 140, 50, 11)</t>
+  </si>
+  <si>
+    <t>(E, 75, 50, 10.2)</t>
+  </si>
+  <si>
+    <t>(F, 140, 50, 11)</t>
+  </si>
+  <si>
+    <t>(D, 75, 50, 10.2)</t>
+  </si>
+  <si>
+    <t>(H, 140, 50, 11)</t>
+  </si>
+  <si>
+    <t>(I, 118, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(C, 118, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(I, 140, 50, 11)</t>
+  </si>
+  <si>
+    <t>(J, 118, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(H, 75, 50, 10.2)</t>
+  </si>
+  <si>
+    <t>(O, 140, 50, 11)</t>
+  </si>
+  <si>
+    <t>(E, 120, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(G, 146, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(L, 138, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(E, 80, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(F, 146, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(L, 97, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(M, 118, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(F, 140, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(K, 151, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(M, 99, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(C, 99, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(J, 211, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(P, 118, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(H, 138, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(I, 97, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(O, 101, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(N, 118, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(I, 211, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(J, 101, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(N, 90, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(P, 85, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(L, 211, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(M, 101, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(Q, 90, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(G, 85, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(L, 142, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(Q, 98, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(K, 142, 50, 13.4)</t>
+  </si>
+  <si>
+    <t>(M, 92, 50, 13.4)</t>
   </si>
 </sst>
 </file>
@@ -588,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B20" sqref="A1:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -908,4 +1101,329 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D991167-6412-F949-8CCA-39D957CAE145}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>